<commit_message>
Update login with data driven
</commit_message>
<xml_diff>
--- a/Data/Excel/Login_Register.xlsx
+++ b/Data/Excel/Login_Register.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>${email}</t>
   </si>
@@ -47,20 +47,29 @@
     <t>rfTest@gmail.com</t>
   </si>
   <si>
-    <t>rf@gmail.com</t>
-  </si>
-  <si>
     <t>rfTest2@gmail.com</t>
   </si>
   <si>
     <t>${confirmPassword}</t>
+  </si>
+  <si>
+    <t>#BLANK</t>
+  </si>
+  <si>
+    <t>someone@notregistered.com</t>
+  </si>
+  <si>
+    <t>TestPassword!</t>
+  </si>
+  <si>
+    <t>email=someone@registereduser.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +90,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -117,6 +132,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -426,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -480,7 +498,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,48 +518,38 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>7</v>
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>123</v>
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>12345678</v>
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>123</v>
-      </c>
+      <c r="A6" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -577,7 +585,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>12345678</v>

</xml_diff>